<commit_message>
added check for missing scale factors
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -440,13 +440,13 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>92.15781616936104</v>
+        <v>94.46899309999804</v>
       </c>
       <c r="D2">
-        <v>22.05185427287049</v>
+        <v>21.57740831269041</v>
       </c>
       <c r="E2">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -457,13 +457,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>61.42295365870407</v>
+        <v>59.65792117753361</v>
       </c>
       <c r="D3">
-        <v>16.3775839809099</v>
+        <v>11.07754467993177</v>
       </c>
       <c r="E3">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -474,13 +474,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1.538521264718646</v>
+        <v>1.584823736996712</v>
       </c>
       <c r="D4">
-        <v>0.2817138177826465</v>
+        <v>0.2047962949222923</v>
       </c>
       <c r="E4">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -490,7 +490,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1786,13 +1786,13 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>83.61339930203907</v>
+        <v>127.3302731060022</v>
       </c>
       <c r="C93">
-        <v>106.4651696844984</v>
+        <v>63.60515352569047</v>
       </c>
       <c r="D93">
-        <v>0.785359188829747</v>
+        <v>2.001886105888774</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1800,13 +1800,13 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>53.18243099411055</v>
+        <v>102.0180055419622</v>
       </c>
       <c r="C94">
-        <v>102.0180055419622</v>
+        <v>61.64959602285769</v>
       </c>
       <c r="D94">
-        <v>0.5213043590842942</v>
+        <v>1.6548041207624</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1814,13 +1814,13 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>61.64959602285769</v>
+        <v>101.3061344100871</v>
       </c>
       <c r="C95">
-        <v>101.3061344100871</v>
+        <v>71.72341537356378</v>
       </c>
       <c r="D95">
-        <v>0.6085475117755479</v>
+        <v>1.412455526308178</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1828,13 +1828,13 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>71.72341537356378</v>
+        <v>140.3276247977545</v>
       </c>
       <c r="C96">
-        <v>140.3276247977545</v>
+        <v>77.79176337404951</v>
       </c>
       <c r="D96">
-        <v>0.5111140124899448</v>
+        <v>1.80388795306016</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1842,13 +1842,13 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>77.79176337404951</v>
+        <v>118.9087148324145</v>
       </c>
       <c r="C97">
-        <v>118.9087148324145</v>
+        <v>73.96518692076563</v>
       </c>
       <c r="D97">
-        <v>0.6542141464037041</v>
+        <v>1.607630829890204</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1856,13 +1856,13 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>73.96518692076563</v>
+        <v>79.81990457630535</v>
       </c>
       <c r="C98">
-        <v>124.2678220707664</v>
+        <v>53.9141290132487</v>
       </c>
       <c r="D98">
-        <v>0.5952078799501688</v>
+        <v>1.480500678341491</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1870,13 +1870,13 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>49.59522849796931</v>
+        <v>69.41246711087447</v>
       </c>
       <c r="C99">
-        <v>33.49895695659366</v>
+        <v>55.22297405571379</v>
       </c>
       <c r="D99">
-        <v>1.480500678341491</v>
+        <v>1.256949092253617</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1884,13 +1884,13 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>43.12868056213535</v>
+        <v>118.7535901515417</v>
       </c>
       <c r="C100">
-        <v>34.31219357086994</v>
+        <v>69.04138577580339</v>
       </c>
       <c r="D100">
-        <v>1.256949092253617</v>
+        <v>1.720034857602188</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1898,13 +1898,13 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>118.7535901515417</v>
+        <v>69.96164632591756</v>
       </c>
       <c r="C101">
-        <v>69.04138577580339</v>
+        <v>49.53083258510415</v>
       </c>
       <c r="D101">
-        <v>1.720034857602188</v>
+        <v>1.412486781959683</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1912,13 +1912,13 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>69.96164632591756</v>
+        <v>92.04173623567482</v>
       </c>
       <c r="C102">
-        <v>49.53083258510415</v>
+        <v>56.64580027190066</v>
       </c>
       <c r="D102">
-        <v>1.412486781959683</v>
+        <v>1.62486425814223</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1926,13 +1926,13 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>92.04173623567482</v>
+        <v>86.74587625934981</v>
       </c>
       <c r="C103">
-        <v>56.64580027190066</v>
+        <v>64.66040847130827</v>
       </c>
       <c r="D103">
-        <v>1.62486425814223</v>
+        <v>1.341560907364845</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1940,13 +1940,13 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>86.74587625934981</v>
+        <v>84.95293936120969</v>
       </c>
       <c r="C104">
-        <v>64.66040847130827</v>
+        <v>53.2616494368153</v>
       </c>
       <c r="D104">
-        <v>1.341560907364845</v>
+        <v>1.595011424908836</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1954,13 +1954,13 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>84.95293936120969</v>
+        <v>83.52144730751426</v>
       </c>
       <c r="C105">
-        <v>53.2616494368153</v>
+        <v>54.37586792161703</v>
       </c>
       <c r="D105">
-        <v>1.595011424908836</v>
+        <v>1.536002099826906</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1968,13 +1968,13 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>83.52144730751426</v>
+        <v>81.76012591679945</v>
       </c>
       <c r="C106">
-        <v>54.37586792161703</v>
+        <v>53.89297072047374</v>
       </c>
       <c r="D106">
-        <v>1.536002099826906</v>
+        <v>1.517083300916256</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1982,13 +1982,13 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>81.76012591679945</v>
+        <v>74.70374942138558</v>
       </c>
       <c r="C107">
-        <v>53.89297072047374</v>
+        <v>49.89816386360129</v>
       </c>
       <c r="D107">
-        <v>1.517083300916256</v>
+        <v>1.497124215343703</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1996,13 +1996,13 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>74.70374942138558</v>
+        <v>82.5651905570128</v>
       </c>
       <c r="C108">
-        <v>49.89816386360129</v>
+        <v>60.24301805276964</v>
       </c>
       <c r="D108">
-        <v>1.497124215343703</v>
+        <v>1.370535428432389</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2010,13 +2010,13 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>82.5651905570128</v>
+        <v>95.21899376075842</v>
       </c>
       <c r="C109">
-        <v>60.24301805276964</v>
+        <v>59.94789432058433</v>
       </c>
       <c r="D109">
-        <v>1.370535428432389</v>
+        <v>1.588362607893353</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2024,13 +2024,13 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>95.21899376075842</v>
+        <v>80.16003887249099</v>
       </c>
       <c r="C110">
-        <v>59.94789432058433</v>
+        <v>67.07701612277917</v>
       </c>
       <c r="D110">
-        <v>1.588362607893353</v>
+        <v>1.195044793372507</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2038,13 +2038,13 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>80.16003887249099</v>
+        <v>78.59409323895534</v>
       </c>
       <c r="C111">
-        <v>67.07701612277917</v>
+        <v>49.55871698610288</v>
       </c>
       <c r="D111">
-        <v>1.195044793372507</v>
+        <v>1.5858782877893</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2052,13 +2052,13 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>78.59409323895534</v>
+        <v>83.15942755747569</v>
       </c>
       <c r="C112">
-        <v>49.55871698610288</v>
+        <v>48.03406110168184</v>
       </c>
       <c r="D112">
-        <v>1.5858782877893</v>
+        <v>1.731259561448241</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2066,13 +2066,13 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>83.15942755747569</v>
+        <v>78.13976942236754</v>
       </c>
       <c r="C113">
-        <v>48.03406110168184</v>
+        <v>51.22571652023375</v>
       </c>
       <c r="D113">
-        <v>1.731259561448241</v>
+        <v>1.525401199444481</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2080,13 +2080,13 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>78.13976942236754</v>
+        <v>67.88175430094499</v>
       </c>
       <c r="C114">
-        <v>51.22571652023375</v>
+        <v>52.80135691785801</v>
       </c>
       <c r="D114">
-        <v>1.525401199444481</v>
+        <v>1.285606246948298</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2094,13 +2094,13 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>67.88175430094499</v>
+        <v>109.4123045117918</v>
       </c>
       <c r="C115">
-        <v>52.80135691785801</v>
+        <v>55.68839430941462</v>
       </c>
       <c r="D115">
-        <v>1.285606246948298</v>
+        <v>1.964723635303212</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2108,13 +2108,13 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>109.4123045117918</v>
+        <v>76.59986884740009</v>
       </c>
       <c r="C116">
-        <v>55.68839430941462</v>
+        <v>55.97766548372164</v>
       </c>
       <c r="D116">
-        <v>1.964723635303212</v>
+        <v>1.368400560928633</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2122,13 +2122,13 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>76.59986884740009</v>
+        <v>75.24309296985116</v>
       </c>
       <c r="C117">
-        <v>55.97766548372164</v>
+        <v>51.56877466101838</v>
       </c>
       <c r="D117">
-        <v>1.368400560928633</v>
+        <v>1.459082428552031</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2136,13 +2136,13 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>75.24309296985116</v>
+        <v>75.11842308285757</v>
       </c>
       <c r="C118">
-        <v>51.56877466101838</v>
+        <v>47.19333436198117</v>
       </c>
       <c r="D118">
-        <v>1.459082428552031</v>
+        <v>1.591716798535278</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2150,13 +2150,13 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>75.11842308285757</v>
+        <v>120.5815489401468</v>
       </c>
       <c r="C119">
-        <v>47.19333436198117</v>
+        <v>58.11715443574836</v>
       </c>
       <c r="D119">
-        <v>1.591716798535278</v>
+        <v>2.07480132347939</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2164,13 +2164,13 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>120.5815489401468</v>
+        <v>83.95941132988374</v>
       </c>
       <c r="C120">
-        <v>58.11715443574836</v>
+        <v>50.30705132512806</v>
       </c>
       <c r="D120">
-        <v>2.07480132347939</v>
+        <v>1.668939226576107</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2178,13 +2178,13 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>83.95941132988374</v>
+        <v>86.43158803430291</v>
       </c>
       <c r="C121">
-        <v>50.30705132512806</v>
+        <v>55.55044377704145</v>
       </c>
       <c r="D121">
-        <v>1.668939226576107</v>
+        <v>1.555911747189757</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2192,13 +2192,13 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>86.43158803430291</v>
+        <v>147.3345890609781</v>
       </c>
       <c r="C122">
-        <v>55.55044377704145</v>
+        <v>94.09506976384151</v>
       </c>
       <c r="D122">
-        <v>1.555911747189757</v>
+        <v>1.565805620111196</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2206,13 +2206,13 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>147.3345890609781</v>
+        <v>83.29000154297175</v>
       </c>
       <c r="C123">
-        <v>94.09506976384151</v>
+        <v>60.31823792624595</v>
       </c>
       <c r="D123">
-        <v>1.565805620111196</v>
+        <v>1.380842750161477</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2220,13 +2220,13 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>83.29000154297175</v>
+        <v>85.94645549922355</v>
       </c>
       <c r="C124">
-        <v>60.31823792624595</v>
+        <v>53.53695296428278</v>
       </c>
       <c r="D124">
-        <v>1.380842750161477</v>
+        <v>1.605366961331602</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2234,13 +2234,13 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>85.94645549922355</v>
+        <v>111.9665666935077</v>
       </c>
       <c r="C125">
-        <v>53.53695296428278</v>
+        <v>73.12615160391438</v>
       </c>
       <c r="D125">
-        <v>1.605366961331602</v>
+        <v>1.531142610922168</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -2248,13 +2248,13 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>111.9665666935077</v>
+        <v>71.10298856978135</v>
       </c>
       <c r="C126">
-        <v>73.12615160391438</v>
+        <v>48.11801401165371</v>
       </c>
       <c r="D126">
-        <v>1.531142610922168</v>
+        <v>1.477679202482482</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2262,13 +2262,13 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>71.10298856978135</v>
+        <v>81.35050890914071</v>
       </c>
       <c r="C127">
-        <v>48.11801401165371</v>
+        <v>48.56890304104873</v>
       </c>
       <c r="D127">
-        <v>1.477679202482482</v>
+        <v>1.674950509802252</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2276,13 +2276,13 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>81.35050890914071</v>
+        <v>88.99591112482641</v>
       </c>
       <c r="C128">
-        <v>48.56890304104873</v>
+        <v>53.90950470606387</v>
       </c>
       <c r="D128">
-        <v>1.674950509802252</v>
+        <v>1.65083896819434</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -2290,13 +2290,13 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>88.99591112482641</v>
+        <v>91.04873018252496</v>
       </c>
       <c r="C129">
-        <v>53.90950470606387</v>
+        <v>57.53929895116643</v>
       </c>
       <c r="D129">
-        <v>1.65083896819434</v>
+        <v>1.582374687251542</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2304,13 +2304,13 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>91.04873018252496</v>
+        <v>76.0523067427866</v>
       </c>
       <c r="C130">
-        <v>57.53929895116643</v>
+        <v>60.30145810831662</v>
       </c>
       <c r="D130">
-        <v>1.582374687251542</v>
+        <v>1.261201787296378</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -2318,13 +2318,13 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>76.0523067427866</v>
+        <v>110.6644519564786</v>
       </c>
       <c r="C131">
-        <v>60.30145810831662</v>
+        <v>59.17088408170569</v>
       </c>
       <c r="D131">
-        <v>1.261201787296378</v>
+        <v>1.870251791466702</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2332,13 +2332,13 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>110.6644519564786</v>
+        <v>83.74275648431616</v>
       </c>
       <c r="C132">
-        <v>59.17088408170569</v>
+        <v>60.90453017153631</v>
       </c>
       <c r="D132">
-        <v>1.870251791466702</v>
+        <v>1.374984032361082</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2346,13 +2346,13 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>83.74275648431616</v>
+        <v>80.19615028544978</v>
       </c>
       <c r="C133">
-        <v>60.90453017153631</v>
+        <v>48.95309365838605</v>
       </c>
       <c r="D133">
-        <v>1.374984032361082</v>
+        <v>1.638224355034435</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -2360,13 +2360,13 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>80.19615028544978</v>
+        <v>151.2924545550028</v>
       </c>
       <c r="C134">
-        <v>48.95309365838605</v>
+        <v>82.75858491948337</v>
       </c>
       <c r="D134">
-        <v>1.638224355034435</v>
+        <v>1.828117949360742</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -2374,13 +2374,13 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>151.2924545550028</v>
+        <v>81.32725951054034</v>
       </c>
       <c r="C135">
-        <v>82.75858491948337</v>
+        <v>60.44584443905985</v>
       </c>
       <c r="D135">
-        <v>1.828117949360742</v>
+        <v>1.345456586226249</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -2388,13 +2388,13 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>81.32725951054034</v>
+        <v>119.6782903872859</v>
       </c>
       <c r="C136">
-        <v>60.44584443905985</v>
+        <v>71.70266934115105</v>
       </c>
       <c r="D136">
-        <v>1.345456586226249</v>
+        <v>1.669091143843944</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2402,13 +2402,13 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>119.6782903872859</v>
+        <v>90.82230840747037</v>
       </c>
       <c r="C137">
-        <v>71.70266934115105</v>
+        <v>54.04126259227419</v>
       </c>
       <c r="D137">
-        <v>1.669091143843944</v>
+        <v>1.680610408618662</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -2416,26 +2416,12 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>90.82230840747037</v>
+        <v>74.86931803790995</v>
       </c>
       <c r="C138">
-        <v>54.04126259227419</v>
+        <v>55.36960151499506</v>
       </c>
       <c r="D138">
-        <v>1.680610408618662</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139">
-        <v>74.86931803790995</v>
-      </c>
-      <c r="C139">
-        <v>55.36960151499506</v>
-      </c>
-      <c r="D139">
         <v>1.352173683562343</v>
       </c>
     </row>
@@ -7051,11 +7037,14 @@
       <c r="D248">
         <v>518.48</v>
       </c>
+      <c r="E248">
+        <v>100</v>
+      </c>
       <c r="F248">
-        <v>0.1612663927288209</v>
+        <v>0.1928714704520907</v>
       </c>
       <c r="G248">
-        <v>83.61339930203907</v>
+        <v>100</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -7069,10 +7058,10 @@
         <v>660.182</v>
       </c>
       <c r="F249">
-        <v>0.1612663927288209</v>
+        <v>0.1928714704520907</v>
       </c>
       <c r="G249">
-        <v>106.4651696844984</v>
+        <v>127.3302731060022</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -7086,10 +7075,10 @@
         <v>329.78</v>
       </c>
       <c r="F250">
-        <v>0.1612663927288209</v>
+        <v>0.1928714704520907</v>
       </c>
       <c r="G250">
-        <v>53.18243099411055</v>
+        <v>63.60515352569047</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -7310,11 +7299,14 @@
       <c r="D262">
         <v>773.812</v>
       </c>
+      <c r="E262">
+        <v>200</v>
+      </c>
       <c r="F262">
-        <v>0.1605917484747799</v>
+        <v>0.258460711387262</v>
       </c>
       <c r="G262">
-        <v>124.2678220707664</v>
+        <v>200</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -7328,10 +7320,10 @@
         <v>308.828</v>
       </c>
       <c r="F263">
-        <v>0.1605917484747799</v>
+        <v>0.258460711387262</v>
       </c>
       <c r="G263">
-        <v>49.59522849796931</v>
+        <v>79.81990457630535</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -7345,10 +7337,10 @@
         <v>208.597</v>
       </c>
       <c r="F264">
-        <v>0.1605917484747799</v>
+        <v>0.258460711387262</v>
       </c>
       <c r="G264">
-        <v>33.49895695659366</v>
+        <v>53.9141290132487</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -7362,10 +7354,10 @@
         <v>268.561</v>
       </c>
       <c r="F265">
-        <v>0.1605917484747799</v>
+        <v>0.258460711387262</v>
       </c>
       <c r="G265">
-        <v>43.12868056213535</v>
+        <v>69.41246711087447</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -7379,10 +7371,10 @@
         <v>213.661</v>
       </c>
       <c r="F266">
-        <v>0.1605917484747799</v>
+        <v>0.258460711387262</v>
       </c>
       <c r="G266">
-        <v>34.31219357086994</v>
+        <v>55.22297405571379</v>
       </c>
     </row>
     <row r="267" spans="1:7">

</xml_diff>